<commit_message>
Added new corp testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/HotelsScripts_Skytravelers.xlsx
+++ b/src/test/resources/testdata/HotelsScripts_Skytravelers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationScripts\Auto\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EF02C4-46EE-41B0-9CA0-88D8676FB5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915AFD9C-3AA5-4BB9-9478-36243E05603A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="5" activeTab="8" xr2:uid="{512D99D7-B637-4054-871A-E0DB86511A8A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="4" activeTab="8" xr2:uid="{512D99D7-B637-4054-871A-E0DB86511A8A}"/>
   </bookViews>
   <sheets>
     <sheet name="TCHO_1" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="232">
   <si>
     <t>TestRun</t>
   </si>
@@ -421,63 +421,6 @@
     <t>kengeri</t>
   </si>
   <si>
-    <t>Doordie@101</t>
-  </si>
-  <si>
-    <t>Doordie@102</t>
-  </si>
-  <si>
-    <t>Doordie@103</t>
-  </si>
-  <si>
-    <t>Doordie@104</t>
-  </si>
-  <si>
-    <t>Doordie@105</t>
-  </si>
-  <si>
-    <t>Doordie@106</t>
-  </si>
-  <si>
-    <t>Doordie@107</t>
-  </si>
-  <si>
-    <t>Doordie@108</t>
-  </si>
-  <si>
-    <t>Doordie@109</t>
-  </si>
-  <si>
-    <t>Doordie@110</t>
-  </si>
-  <si>
-    <t>Doordie@111</t>
-  </si>
-  <si>
-    <t>Doordie@112</t>
-  </si>
-  <si>
-    <t>Doordie@113</t>
-  </si>
-  <si>
-    <t>Doordie@114</t>
-  </si>
-  <si>
-    <t>Doordie@115</t>
-  </si>
-  <si>
-    <t>Doordie@116</t>
-  </si>
-  <si>
-    <t>Doordie@117</t>
-  </si>
-  <si>
-    <t>Doordie@118</t>
-  </si>
-  <si>
-    <t>Doordie@119</t>
-  </si>
-  <si>
     <t>hyderabad</t>
   </si>
   <si>
@@ -707,13 +650,103 @@
   </si>
   <si>
     <t>rajarajeswari nagar</t>
+  </si>
+  <si>
+    <t>https://neo.tripgain.com/login</t>
+  </si>
+  <si>
+    <t>testtraveller98@tripgain.com</t>
+  </si>
+  <si>
+    <t>@AM@TGA1$29TN</t>
+  </si>
+  <si>
+    <t>UserName1</t>
+  </si>
+  <si>
+    <t>Password1</t>
+  </si>
+  <si>
+    <t>automation@tga.com</t>
+  </si>
+  <si>
+    <t>SearchBy</t>
+  </si>
+  <si>
+    <t>SearchValue</t>
+  </si>
+  <si>
+    <t>testapprover98@tripgain.com</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Reject</t>
+  </si>
+  <si>
+    <t>TravellerSearchValue</t>
+  </si>
+  <si>
+    <t>TravellerSearchValue2</t>
+  </si>
+  <si>
+    <t>testfinance98@tripgain.com</t>
+  </si>
+  <si>
+    <t>Status2</t>
+  </si>
+  <si>
+    <t>Approve</t>
+  </si>
+  <si>
+    <t>tirupati</t>
+  </si>
+  <si>
+    <t>Rajkot</t>
+  </si>
+  <si>
+    <t>Vadodara</t>
+  </si>
+  <si>
+    <t>visakhapatnam</t>
+  </si>
+  <si>
+    <t>ludhiana</t>
+  </si>
+  <si>
+    <t>satara</t>
+  </si>
+  <si>
+    <t>solapur</t>
+  </si>
+  <si>
+    <t>Amritsar</t>
+  </si>
+  <si>
+    <t>varanasi</t>
+  </si>
+  <si>
+    <t>udaipur</t>
+  </si>
+  <si>
+    <t>puri</t>
+  </si>
+  <si>
+    <t>bhuvaneswar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -755,6 +788,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF667085"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF667085"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -777,7 +834,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -786,6 +843,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4573,10 +4639,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA9BB05B-65AF-4EA0-B284-D37B978614F7}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B1" sqref="B1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4584,10 +4650,16 @@
     <col min="1" max="1" width="39.6328125" customWidth="1"/>
     <col min="2" max="2" width="29.81640625" customWidth="1"/>
     <col min="3" max="3" width="20.36328125" customWidth="1"/>
-    <col min="4" max="4" width="43.81640625" customWidth="1"/>
+    <col min="4" max="4" width="30.453125" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" customWidth="1"/>
+    <col min="6" max="6" width="23.1796875" customWidth="1"/>
+    <col min="7" max="7" width="21.453125" customWidth="1"/>
+    <col min="9" max="9" width="28.08984375" customWidth="1"/>
+    <col min="12" max="12" width="27.7265625" customWidth="1"/>
+    <col min="13" max="13" width="26.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4601,21 +4673,48 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="F1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H1" t="s">
+        <v>208</v>
+      </c>
+      <c r="I1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J1" t="s">
+        <v>211</v>
+      </c>
+      <c r="K1" t="s">
+        <v>213</v>
+      </c>
+      <c r="L1" t="s">
+        <v>215</v>
+      </c>
+      <c r="M1" t="s">
+        <v>216</v>
+      </c>
+      <c r="N1" t="s">
+        <v>218</v>
+      </c>
+      <c r="O1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>122</v>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>123</v>
+        <v>204</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>124</v>
@@ -4623,16 +4722,43 @@
       <c r="E2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>122</v>
+      <c r="F2" t="s">
+        <v>207</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>125</v>
+        <v>204</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>39</v>
@@ -4640,16 +4766,46 @@
       <c r="E3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>122</v>
+      <c r="F3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>126</v>
+        <v>204</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>49</v>
@@ -4657,16 +4813,46 @@
       <c r="E4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>122</v>
+      <c r="F4" t="s">
+        <v>207</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>127</v>
+        <v>204</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>47</v>
@@ -4674,33 +4860,93 @@
       <c r="E5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>122</v>
+      <c r="F5" t="s">
+        <v>207</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>128</v>
+        <v>204</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>122</v>
+      <c r="F6" t="s">
+        <v>207</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>129</v>
+        <v>204</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>48</v>
@@ -4708,33 +4954,93 @@
       <c r="E7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>122</v>
+      <c r="F7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>130</v>
+        <v>204</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="E8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>122</v>
+      <c r="F8" t="s">
+        <v>207</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>131</v>
+        <v>204</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>42</v>
@@ -4742,50 +5048,140 @@
       <c r="E9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>122</v>
+      <c r="F9" t="s">
+        <v>207</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>132</v>
+        <v>204</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>122</v>
+      <c r="F10" t="s">
+        <v>207</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>133</v>
+        <v>204</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>122</v>
+      <c r="F11" t="s">
+        <v>207</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>134</v>
+        <v>204</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>87</v>
@@ -4793,152 +5189,422 @@
       <c r="E12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>122</v>
+      <c r="F12" t="s">
+        <v>207</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>135</v>
+        <v>204</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="E13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>122</v>
+      <c r="F13" t="s">
+        <v>207</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N13" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>136</v>
+        <v>204</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>122</v>
+      <c r="F14" t="s">
+        <v>207</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N14" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>137</v>
+        <v>204</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>122</v>
+      <c r="F15" t="s">
+        <v>207</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N15" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>138</v>
+        <v>204</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="E16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>122</v>
+      <c r="F16" t="s">
+        <v>207</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N16" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>139</v>
+        <v>204</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="E17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>122</v>
+      <c r="F17" t="s">
+        <v>207</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N17" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>140</v>
+        <v>204</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="E18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>122</v>
+      <c r="F18" t="s">
+        <v>207</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N18" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>141</v>
+        <v>204</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>122</v>
+      <c r="F19" t="s">
+        <v>207</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N19" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>142</v>
+        <v>204</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="E20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>122</v>
+      <c r="F20" t="s">
+        <v>207</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N20" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>143</v>
+        <v>204</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>88</v>
@@ -4946,91 +5612,177 @@
       <c r="E21">
         <v>2</v>
       </c>
+      <c r="F21" t="s">
+        <v>207</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L21" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M21" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N21" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D22" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D23" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D24" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D25" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D26" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D27" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D28" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D29" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D30" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D31" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D32" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D33" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D34" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D35" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D36" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D37" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D38" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D39" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D40" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D41" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D42" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D43" s="1" t="s">
+        <v>231</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{421CF4A1-C060-4815-9917-6B79275BB28C}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{99712185-1D17-4F41-8CA1-CC85B20E7905}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{35AB73B7-07C9-442E-ADA6-F5F9EA2123B3}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{93BB6483-3FE5-42F3-ABF1-7D012216F2E0}"/>
-    <hyperlink ref="B4" r:id="rId5" xr:uid="{A72E097C-3615-48D5-AE1B-AE2546DF7D70}"/>
-    <hyperlink ref="B5" r:id="rId6" xr:uid="{106FE48F-75F5-410F-B37F-29F039DA3415}"/>
-    <hyperlink ref="B6" r:id="rId7" xr:uid="{8B59CBCC-B34E-425C-93A2-34A1E240AD50}"/>
-    <hyperlink ref="B7" r:id="rId8" xr:uid="{E8842F99-A9C1-42D2-A816-BD2F4F1C676A}"/>
-    <hyperlink ref="B8" r:id="rId9" xr:uid="{25766F75-5F8F-40FF-84F2-0634F77BC15C}"/>
-    <hyperlink ref="B9" r:id="rId10" xr:uid="{0FA405BE-A79C-4D33-8811-0D47A65C885E}"/>
-    <hyperlink ref="B10" r:id="rId11" xr:uid="{C68BA698-50E2-4DD6-BB22-F971A3B3E023}"/>
-    <hyperlink ref="B11" r:id="rId12" xr:uid="{32891291-5A57-4334-8B74-D060FB6EAD81}"/>
-    <hyperlink ref="B12" r:id="rId13" xr:uid="{F71B49FB-CB1A-4CD0-BD55-D46142E15DE1}"/>
-    <hyperlink ref="B13" r:id="rId14" xr:uid="{53AE0A71-5A85-4583-ABAD-21E05CA4071C}"/>
-    <hyperlink ref="B14" r:id="rId15" xr:uid="{FCC406FD-2CDB-4664-8016-8DE482D3EDD5}"/>
-    <hyperlink ref="B15" r:id="rId16" xr:uid="{B18383EF-F842-4450-9520-735DB0167D95}"/>
-    <hyperlink ref="B16" r:id="rId17" xr:uid="{8AF918A9-301A-4509-8C7F-38D515A921AD}"/>
-    <hyperlink ref="B17" r:id="rId18" xr:uid="{69605BF0-2D65-47D8-81CF-33ABEAFDFB17}"/>
-    <hyperlink ref="B18" r:id="rId19" xr:uid="{58366A44-2980-42D4-A87C-0A23AD30C073}"/>
-    <hyperlink ref="B19" r:id="rId20" xr:uid="{DB49D9D5-2E21-4622-A927-F1FFABDB4FCD}"/>
-    <hyperlink ref="A3" r:id="rId21" xr:uid="{E9414D7A-2EBE-4F42-B484-E4A015640296}"/>
-    <hyperlink ref="A4" r:id="rId22" xr:uid="{DC83B4AB-379E-4F5B-A3CB-FD784D550137}"/>
-    <hyperlink ref="A5" r:id="rId23" xr:uid="{9AE1C327-2E2B-4ED0-A34D-E911F6F67933}"/>
-    <hyperlink ref="A6" r:id="rId24" xr:uid="{2A7F8886-ECDA-4AA7-8BD6-1BF597E467CD}"/>
-    <hyperlink ref="A7" r:id="rId25" xr:uid="{50D5CB16-EF6B-4654-8EFF-B5BA613F9C39}"/>
-    <hyperlink ref="A8" r:id="rId26" xr:uid="{0064AD75-5498-4821-9877-533ABE97CC94}"/>
-    <hyperlink ref="A9" r:id="rId27" xr:uid="{7FE5597F-C3E0-438D-B37D-852A45977874}"/>
-    <hyperlink ref="A10" r:id="rId28" xr:uid="{429E4E09-D4E5-43E9-BD5E-0FB2B916D46B}"/>
-    <hyperlink ref="A11" r:id="rId29" xr:uid="{A2B01F78-79FD-4C00-B3A0-E53FAA93D251}"/>
-    <hyperlink ref="A12" r:id="rId30" xr:uid="{717C3E1F-F100-4B71-B387-D4E9B6978815}"/>
-    <hyperlink ref="A13" r:id="rId31" xr:uid="{07815760-B9F7-419B-AAA5-5C1D1EA218FE}"/>
-    <hyperlink ref="A14" r:id="rId32" xr:uid="{B0BC493E-8792-4FE5-B71C-15FDDA591563}"/>
-    <hyperlink ref="A15" r:id="rId33" xr:uid="{8CFF825D-FD4F-49DE-B049-8586E2CEDBB6}"/>
-    <hyperlink ref="A16" r:id="rId34" xr:uid="{DE8AC35D-B9BE-450E-9409-0D6293216B43}"/>
-    <hyperlink ref="A17" r:id="rId35" xr:uid="{A1592D7B-424E-4222-B956-9948CF6CB75F}"/>
-    <hyperlink ref="A18" r:id="rId36" xr:uid="{81632CFA-81E0-404D-B081-65C043DBA07A}"/>
-    <hyperlink ref="A19" r:id="rId37" xr:uid="{44D73D2D-0B2A-4E93-82FE-0E108DFA2B9A}"/>
-    <hyperlink ref="C3" r:id="rId38" display="Doordie@100" xr:uid="{A112D8C5-632D-4163-85AF-D74CC3E7061C}"/>
-    <hyperlink ref="C4" r:id="rId39" display="Doordie@100" xr:uid="{262BEE6C-82F6-4561-8631-C95CD3EA2254}"/>
-    <hyperlink ref="C5" r:id="rId40" display="Doordie@100" xr:uid="{7C60ABA3-5B9F-49B6-ADF1-B3C730E753AD}"/>
-    <hyperlink ref="C6" r:id="rId41" display="Doordie@100" xr:uid="{5E8C98B0-15CF-4107-B20B-59C707678720}"/>
-    <hyperlink ref="C7" r:id="rId42" display="Doordie@100" xr:uid="{E12CF9A3-2766-4AE4-A8EC-AAB807D734C5}"/>
-    <hyperlink ref="C8" r:id="rId43" display="Doordie@100" xr:uid="{086E5345-8096-4F2E-8484-2CA63A6338B5}"/>
-    <hyperlink ref="C9" r:id="rId44" display="Doordie@100" xr:uid="{8FF4D999-170A-49C8-A95D-038EAFE9807D}"/>
-    <hyperlink ref="C10" r:id="rId45" display="Doordie@100" xr:uid="{36987A20-7E5E-4D7A-B8B4-5F0F72540D10}"/>
-    <hyperlink ref="C11" r:id="rId46" display="Doordie@100" xr:uid="{F29E61B6-090D-4BB0-9C63-66795D5D6404}"/>
-    <hyperlink ref="C12" r:id="rId47" display="Doordie@100" xr:uid="{2763913D-E109-43A3-B959-FCD2F9234438}"/>
-    <hyperlink ref="C13" r:id="rId48" display="Doordie@100" xr:uid="{5AACEC40-7D66-4DC7-944D-1BD8C44C4693}"/>
-    <hyperlink ref="C14" r:id="rId49" display="Doordie@100" xr:uid="{6E4A8AED-36E0-4A11-9D7F-FED15F3683CC}"/>
-    <hyperlink ref="C15" r:id="rId50" display="Doordie@100" xr:uid="{CF75446F-BA0B-4C33-B213-4E1033D0C505}"/>
-    <hyperlink ref="C16" r:id="rId51" display="Doordie@100" xr:uid="{7A1CDF89-EBD0-41C1-A27E-178663425F1D}"/>
-    <hyperlink ref="C17" r:id="rId52" display="Doordie@100" xr:uid="{D67C095E-3233-454C-81B4-7C79E945566E}"/>
-    <hyperlink ref="C18" r:id="rId53" display="Doordie@100" xr:uid="{3C02E397-C7A7-4497-974A-EB4B88830A53}"/>
-    <hyperlink ref="C19" r:id="rId54" display="Doordie@100" xr:uid="{A16BBD27-16CD-454E-B431-67BBA0106389}"/>
-    <hyperlink ref="B20" r:id="rId55" xr:uid="{5E51053F-C15A-4D73-8AA3-394EE53F0048}"/>
-    <hyperlink ref="A20" r:id="rId56" xr:uid="{DB373907-56EE-4073-A331-0139B2D2E8D7}"/>
-    <hyperlink ref="C20" r:id="rId57" display="Doordie@100" xr:uid="{894BD5D1-E222-4454-BF47-F8B6C7CF3822}"/>
-    <hyperlink ref="B21" r:id="rId58" xr:uid="{F329B2B6-6CFA-4FB8-9B1E-9BB823CEEC0E}"/>
-    <hyperlink ref="A21" r:id="rId59" xr:uid="{F9B22ABE-76C2-4ED5-ACB8-2C3213D853F5}"/>
-    <hyperlink ref="C21" r:id="rId60" display="Doordie@100" xr:uid="{7FCFDB99-A1A6-41F3-A2E4-BDF09DADF1EC}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D32C639-9751-46C8-AB5C-5BEC34FB1F52}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="38.81640625" customWidth="1"/>
+    <col min="2" max="2" width="34.08984375" customWidth="1"/>
     <col min="3" max="3" width="18.453125" customWidth="1"/>
     <col min="4" max="4" width="13.81640625" customWidth="1"/>
     <col min="5" max="5" width="15.54296875" customWidth="1"/>
+    <col min="6" max="6" width="19.90625" customWidth="1"/>
+    <col min="7" max="8" width="15.54296875" customWidth="1"/>
+    <col min="9" max="9" width="27.36328125" customWidth="1"/>
+    <col min="10" max="11" width="14.7265625" customWidth="1"/>
+    <col min="12" max="13" width="33.08984375" customWidth="1"/>
+    <col min="14" max="14" width="17.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -5044,416 +5796,978 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="F1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H1" t="s">
+        <v>208</v>
+      </c>
+      <c r="I1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J1" t="s">
+        <v>211</v>
+      </c>
+      <c r="K1" t="s">
+        <v>213</v>
+      </c>
+      <c r="L1" t="s">
+        <v>215</v>
+      </c>
+      <c r="M1" t="s">
+        <v>216</v>
+      </c>
+      <c r="N1" t="s">
+        <v>218</v>
+      </c>
+      <c r="O1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>122</v>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>123</v>
+        <v>204</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="E2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>122</v>
+        <v>140</v>
+      </c>
+      <c r="F2" t="s">
+        <v>207</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>125</v>
+        <v>204</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>122</v>
+        <v>141</v>
+      </c>
+      <c r="F3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>126</v>
+        <v>204</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
+      </c>
+      <c r="F4" t="s">
+        <v>207</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>127</v>
+        <v>204</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>122</v>
+        <v>142</v>
+      </c>
+      <c r="F5" t="s">
+        <v>207</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>128</v>
+        <v>204</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>122</v>
+        <v>145</v>
+      </c>
+      <c r="F6" t="s">
+        <v>207</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>129</v>
+        <v>204</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>122</v>
+        <v>143</v>
+      </c>
+      <c r="F7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>130</v>
+        <v>204</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>122</v>
+        <v>146</v>
+      </c>
+      <c r="F8" t="s">
+        <v>207</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>131</v>
+        <v>204</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="E9" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>122</v>
+        <v>148</v>
+      </c>
+      <c r="F9" t="s">
+        <v>207</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>132</v>
+        <v>204</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="E10" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>122</v>
+        <v>150</v>
+      </c>
+      <c r="F10" t="s">
+        <v>207</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>133</v>
+        <v>204</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="E11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>122</v>
+        <v>152</v>
+      </c>
+      <c r="F11" t="s">
+        <v>207</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>134</v>
+        <v>204</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>122</v>
+        <v>153</v>
+      </c>
+      <c r="F12" t="s">
+        <v>207</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>135</v>
+        <v>204</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="E13" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>122</v>
+        <v>155</v>
+      </c>
+      <c r="F13" t="s">
+        <v>207</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N13" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>136</v>
+        <v>204</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E14" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>122</v>
+        <v>157</v>
+      </c>
+      <c r="F14" t="s">
+        <v>207</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N14" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>137</v>
+        <v>204</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="E15" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>122</v>
+        <v>159</v>
+      </c>
+      <c r="F15" t="s">
+        <v>207</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N15" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>138</v>
+        <v>204</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="E16" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>122</v>
+        <v>160</v>
+      </c>
+      <c r="F16" t="s">
+        <v>207</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N16" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>139</v>
+        <v>204</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="E17" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>122</v>
+        <v>162</v>
+      </c>
+      <c r="F17" t="s">
+        <v>207</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N17" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>140</v>
+        <v>204</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>122</v>
+        <v>156</v>
+      </c>
+      <c r="F18" t="s">
+        <v>207</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N18" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>141</v>
+        <v>204</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="E19" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>122</v>
+        <v>164</v>
+      </c>
+      <c r="F19" t="s">
+        <v>207</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N19" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>142</v>
+        <v>204</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>122</v>
+        <v>165</v>
+      </c>
+      <c r="F20" t="s">
+        <v>207</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N20" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>143</v>
+        <v>204</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="E21" t="s">
-        <v>186</v>
+        <v>167</v>
+      </c>
+      <c r="F21" t="s">
+        <v>207</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L21" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M21" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N21" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="O21" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{4F99C325-BADD-4539-8FF7-DFF9993CC9B2}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{7ABC8269-BEBA-413F-9FFB-2E2F0051B554}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{6CB65E85-93BE-4CDC-8F12-4040CEC19996}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{28A22044-90D0-499A-8746-046B44AEFF3F}"/>
-    <hyperlink ref="B4" r:id="rId5" xr:uid="{277BD9FA-6222-4AC3-84E2-A24C2C48DA5A}"/>
-    <hyperlink ref="B5" r:id="rId6" xr:uid="{6C604675-9F97-4D10-ABBF-50CABC772C94}"/>
-    <hyperlink ref="B6" r:id="rId7" xr:uid="{4CB2E585-F603-439E-AC19-56B81367A4E5}"/>
-    <hyperlink ref="B7" r:id="rId8" xr:uid="{B230F806-4E39-45AD-A17E-41E4ECC0D055}"/>
-    <hyperlink ref="B8" r:id="rId9" xr:uid="{361652F5-73AA-4CC4-9888-046C5044B9BA}"/>
-    <hyperlink ref="B9" r:id="rId10" xr:uid="{409A400F-C316-4385-813B-4CA57017549D}"/>
-    <hyperlink ref="B10" r:id="rId11" xr:uid="{15568EF4-3090-4A22-A607-4CD5A183B976}"/>
-    <hyperlink ref="B11" r:id="rId12" xr:uid="{B1F3CAD1-0126-4585-B3A7-66AB2C59407F}"/>
-    <hyperlink ref="B12" r:id="rId13" xr:uid="{E910639B-A1A6-4781-908F-1E8176B15E84}"/>
-    <hyperlink ref="B13" r:id="rId14" xr:uid="{6D9812E2-4B53-4A24-A730-A8E5FDE70639}"/>
-    <hyperlink ref="B14" r:id="rId15" xr:uid="{74149AD4-F969-478C-896D-AEBC6858CA9A}"/>
-    <hyperlink ref="B15" r:id="rId16" xr:uid="{B2C5CF3F-4946-4ACB-9E39-0A6F78C22A4B}"/>
-    <hyperlink ref="B16" r:id="rId17" xr:uid="{036CEE2D-AF45-42B1-AB48-0949D74CBFAE}"/>
-    <hyperlink ref="B17" r:id="rId18" xr:uid="{062BDD05-579C-4A7B-9602-F1FBF272B345}"/>
-    <hyperlink ref="B18" r:id="rId19" xr:uid="{98B3CFE0-B7BA-42C3-80FE-A2961ACDA81A}"/>
-    <hyperlink ref="B19" r:id="rId20" xr:uid="{CD0ADD6A-A56F-4F6C-AFB9-8B7F11F93DC5}"/>
-    <hyperlink ref="A3" r:id="rId21" xr:uid="{9C1324AB-BF6B-4E59-9D11-26F6CC4F70A7}"/>
-    <hyperlink ref="A4" r:id="rId22" xr:uid="{497721FE-2A87-44F1-A8FF-E46AA030415F}"/>
-    <hyperlink ref="A5" r:id="rId23" xr:uid="{623D0151-AAFF-4895-923A-6ACCAC416534}"/>
-    <hyperlink ref="A6" r:id="rId24" xr:uid="{A708FA40-1D15-4064-B877-F4C245BEFE38}"/>
-    <hyperlink ref="A7" r:id="rId25" xr:uid="{AE800CC3-DD5B-45FC-9ACA-384276C86E20}"/>
-    <hyperlink ref="A8" r:id="rId26" xr:uid="{382B43C3-5FBA-4FA1-92F2-70381A0DFB75}"/>
-    <hyperlink ref="A9" r:id="rId27" xr:uid="{D9139641-735A-4805-B0AF-F42956EFB364}"/>
-    <hyperlink ref="A10" r:id="rId28" xr:uid="{E9E8B172-08FB-48B9-A092-FCB4FE13DB6E}"/>
-    <hyperlink ref="A11" r:id="rId29" xr:uid="{40753906-66B1-4B92-AF47-3D7D4C2CE0D7}"/>
-    <hyperlink ref="A12" r:id="rId30" xr:uid="{7A3D51B6-4198-4B90-A376-2DA3375BD19E}"/>
-    <hyperlink ref="A13" r:id="rId31" xr:uid="{E27D25D3-D2B8-4672-94F2-4CC9BE0AC9A0}"/>
-    <hyperlink ref="A14" r:id="rId32" xr:uid="{B5247CCE-1CB3-42B3-A0E4-5BB1E907D260}"/>
-    <hyperlink ref="A15" r:id="rId33" xr:uid="{724BA3B9-3DDB-4F82-A177-2314A76CA10C}"/>
-    <hyperlink ref="A16" r:id="rId34" xr:uid="{9D3760B7-42D4-4417-8D72-0E9F43BB1AC6}"/>
-    <hyperlink ref="A17" r:id="rId35" xr:uid="{4296078F-1DF6-44C6-8165-64087A02D880}"/>
-    <hyperlink ref="A18" r:id="rId36" xr:uid="{54988E20-0E8D-48E7-ACA3-ADEB736CBDA6}"/>
-    <hyperlink ref="A19" r:id="rId37" xr:uid="{3A765DFB-A714-46EC-9A42-FF1546847688}"/>
-    <hyperlink ref="C3" r:id="rId38" display="Doordie@100" xr:uid="{AEA7299B-8B6C-4A47-B828-EC2CD1E69A2F}"/>
-    <hyperlink ref="C4" r:id="rId39" display="Doordie@100" xr:uid="{2123834E-2AB0-4FD0-A772-6410CB7B9DDC}"/>
-    <hyperlink ref="C5" r:id="rId40" display="Doordie@100" xr:uid="{915C0A94-390C-434B-8F42-6E12AE1A80EA}"/>
-    <hyperlink ref="C6" r:id="rId41" display="Doordie@100" xr:uid="{CB5B6BEE-3C25-45A1-9C8F-259A3D8DF3DD}"/>
-    <hyperlink ref="C7" r:id="rId42" display="Doordie@100" xr:uid="{EB92853D-1B9A-4CC4-A9AF-8BD0CF635D93}"/>
-    <hyperlink ref="C8" r:id="rId43" display="Doordie@100" xr:uid="{27D02071-2945-432F-A685-A34B38B87FF1}"/>
-    <hyperlink ref="C9" r:id="rId44" display="Doordie@100" xr:uid="{1EC24A2E-1598-497C-B6F8-4DCA908AA5ED}"/>
-    <hyperlink ref="C10" r:id="rId45" display="Doordie@100" xr:uid="{0AE794E9-6E03-46F4-AED0-9C5B42198439}"/>
-    <hyperlink ref="C11" r:id="rId46" display="Doordie@100" xr:uid="{3386A85A-BD1C-4EB3-8A54-6075BB8A7896}"/>
-    <hyperlink ref="C12" r:id="rId47" display="Doordie@100" xr:uid="{0A85EB4E-C79D-44C0-A44D-62C8A115A2C8}"/>
-    <hyperlink ref="C13" r:id="rId48" display="Doordie@100" xr:uid="{4BADA009-DDEA-46A6-8277-F669034CF813}"/>
-    <hyperlink ref="C14" r:id="rId49" display="Doordie@100" xr:uid="{55C4C899-9B25-49B3-A9EA-AEB10110EA05}"/>
-    <hyperlink ref="C15" r:id="rId50" display="Doordie@100" xr:uid="{D6C4D5D9-54E1-4CA0-B62F-717B9F53941F}"/>
-    <hyperlink ref="C16" r:id="rId51" display="Doordie@100" xr:uid="{0D42D67E-2ED6-4047-9699-A71C160124A1}"/>
-    <hyperlink ref="C17" r:id="rId52" display="Doordie@100" xr:uid="{016D6C34-A27E-461E-955A-E8C1B59BC6A3}"/>
-    <hyperlink ref="C18" r:id="rId53" display="Doordie@100" xr:uid="{0912A058-6BC9-4829-BBB0-BB4150EB54FD}"/>
-    <hyperlink ref="C19" r:id="rId54" display="Doordie@100" xr:uid="{0000B1EE-C3DE-4F49-9192-A20721FCA24A}"/>
-    <hyperlink ref="B20" r:id="rId55" xr:uid="{61EE19D2-61C7-4621-89F9-931628FDA0CE}"/>
-    <hyperlink ref="A20" r:id="rId56" xr:uid="{5A193398-5151-422F-AE3D-71AAC9233E3B}"/>
-    <hyperlink ref="C20" r:id="rId57" display="Doordie@100" xr:uid="{AB6997F5-F217-43AC-A562-C1CB83CDF394}"/>
-    <hyperlink ref="B21" r:id="rId58" xr:uid="{9E823B61-1094-4EA3-AB8A-DC61FD51D55A}"/>
-    <hyperlink ref="A21" r:id="rId59" xr:uid="{DFC58A2C-23BA-4B78-A4DF-2CF122095EF1}"/>
-    <hyperlink ref="C21" r:id="rId60" display="Doordie@100" xr:uid="{6454D373-2E82-4E37-92B1-8FB89EB2A214}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5463,7 +6777,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5482,10 +6796,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="F1" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -5502,13 +6816,13 @@
         <v>123</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="E2" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="F2" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -5539,10 +6853,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="D1" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -5553,13 +6867,13 @@
         <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
         <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -5572,408 +6886,530 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D33E6F-A6B1-4616-954D-27E1D6F16508}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.6328125" customWidth="1"/>
-    <col min="4" max="4" width="26.54296875" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" customWidth="1"/>
+    <col min="1" max="1" width="31.453125" customWidth="1"/>
+    <col min="2" max="3" width="26.6328125" customWidth="1"/>
+    <col min="6" max="6" width="26.54296875" customWidth="1"/>
+    <col min="8" max="8" width="17.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>157</v>
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="I1" t="s">
+        <v>200</v>
+      </c>
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>179</v>
+      </c>
+      <c r="G2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>126</v>
+      </c>
+      <c r="J3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>126</v>
+      </c>
+      <c r="I4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" t="s">
+        <v>155</v>
+      </c>
+      <c r="I5" t="s">
+        <v>155</v>
+      </c>
+      <c r="J5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>183</v>
+      </c>
+      <c r="G6" t="s">
+        <v>155</v>
+      </c>
+      <c r="H6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G7" t="s">
+        <v>140</v>
+      </c>
+      <c r="H7" t="s">
+        <v>167</v>
+      </c>
+      <c r="I7" t="s">
+        <v>201</v>
+      </c>
+      <c r="J7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" t="s">
+        <v>155</v>
+      </c>
+      <c r="F8" t="s">
+        <v>185</v>
+      </c>
+      <c r="G8" t="s">
+        <v>194</v>
+      </c>
+      <c r="H8" t="s">
+        <v>163</v>
+      </c>
+      <c r="I8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" t="s">
+        <v>186</v>
+      </c>
+      <c r="G9" t="s">
+        <v>155</v>
+      </c>
+      <c r="H9" t="s">
+        <v>154</v>
+      </c>
+      <c r="I9" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>155</v>
+      </c>
+      <c r="F10" t="s">
         <v>187</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" t="s">
+        <v>195</v>
+      </c>
+      <c r="I10" t="s">
+        <v>196</v>
+      </c>
+      <c r="J10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>188</v>
+      </c>
+      <c r="G11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" t="s">
+        <v>155</v>
+      </c>
+      <c r="I11" t="s">
+        <v>197</v>
+      </c>
+      <c r="J11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" t="s">
+        <v>175</v>
+      </c>
+      <c r="F12" t="s">
+        <v>189</v>
+      </c>
+      <c r="G12" t="s">
+        <v>155</v>
+      </c>
+      <c r="H12" t="s">
+        <v>196</v>
+      </c>
+      <c r="I12" t="s">
+        <v>140</v>
+      </c>
+      <c r="J12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" t="s">
+        <v>190</v>
+      </c>
+      <c r="G13" t="s">
+        <v>125</v>
+      </c>
+      <c r="H13" t="s">
+        <v>140</v>
+      </c>
+      <c r="I13" t="s">
+        <v>194</v>
+      </c>
+      <c r="J13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" t="s">
         <v>191</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G14" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" t="s">
+        <v>199</v>
+      </c>
+      <c r="J14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>177</v>
+      </c>
+      <c r="F15" t="s">
         <v>192</v>
       </c>
-      <c r="G1" t="s">
-        <v>219</v>
-      </c>
-      <c r="H1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="G15" t="s">
+        <v>155</v>
+      </c>
+      <c r="H15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" t="s">
+        <v>154</v>
+      </c>
+      <c r="J15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
+        <v>178</v>
+      </c>
+      <c r="F16" t="s">
+        <v>193</v>
+      </c>
+      <c r="G16" t="s">
+        <v>167</v>
+      </c>
+      <c r="H16" t="s">
+        <v>160</v>
+      </c>
+      <c r="I16" t="s">
         <v>198</v>
       </c>
-      <c r="E2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D3" t="s">
-        <v>199</v>
-      </c>
-      <c r="E3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D4" t="s">
-        <v>200</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>145</v>
-      </c>
-      <c r="G4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C5" t="s">
-        <v>159</v>
-      </c>
-      <c r="D5" t="s">
-        <v>201</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" t="s">
-        <v>174</v>
-      </c>
-      <c r="G5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" t="s">
-        <v>202</v>
-      </c>
-      <c r="E6" t="s">
-        <v>174</v>
-      </c>
-      <c r="F6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C7" t="s">
-        <v>174</v>
-      </c>
-      <c r="D7" t="s">
-        <v>203</v>
-      </c>
-      <c r="E7" t="s">
-        <v>159</v>
-      </c>
-      <c r="F7" t="s">
-        <v>186</v>
-      </c>
-      <c r="G7" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" t="s">
-        <v>174</v>
-      </c>
-      <c r="D8" t="s">
-        <v>204</v>
-      </c>
-      <c r="E8" t="s">
-        <v>213</v>
-      </c>
-      <c r="F8" t="s">
-        <v>182</v>
-      </c>
-      <c r="G8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" t="s">
-        <v>205</v>
-      </c>
-      <c r="E9" t="s">
-        <v>174</v>
-      </c>
-      <c r="F9" t="s">
-        <v>173</v>
-      </c>
-      <c r="G9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" t="s">
-        <v>174</v>
-      </c>
-      <c r="D10" t="s">
-        <v>206</v>
-      </c>
-      <c r="E10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" t="s">
-        <v>214</v>
-      </c>
-      <c r="G10" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" t="s">
-        <v>207</v>
-      </c>
-      <c r="E11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" t="s">
-        <v>174</v>
-      </c>
-      <c r="G11" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C12" t="s">
-        <v>194</v>
-      </c>
-      <c r="D12" t="s">
-        <v>208</v>
-      </c>
-      <c r="E12" t="s">
-        <v>174</v>
-      </c>
-      <c r="F12" t="s">
-        <v>215</v>
-      </c>
-      <c r="G12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" t="s">
-        <v>209</v>
-      </c>
-      <c r="E13" t="s">
-        <v>144</v>
-      </c>
-      <c r="F13" t="s">
-        <v>159</v>
-      </c>
-      <c r="G13" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" t="s">
-        <v>210</v>
-      </c>
-      <c r="E14" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" t="s">
-        <v>196</v>
-      </c>
-      <c r="D15" t="s">
-        <v>211</v>
-      </c>
-      <c r="E15" t="s">
-        <v>174</v>
-      </c>
-      <c r="F15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" t="s">
-        <v>197</v>
-      </c>
-      <c r="D16" t="s">
-        <v>212</v>
-      </c>
-      <c r="E16" t="s">
-        <v>186</v>
-      </c>
-      <c r="F16" t="s">
-        <v>179</v>
-      </c>
-      <c r="G16" t="s">
-        <v>217</v>
+      <c r="J16" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{4D03F68A-C2E4-4D0F-A0D2-08A45B4C5398}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{F7B99411-598A-49BE-934E-C540226F5D84}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{6BF81A2B-86FF-406A-B08E-B8045FAC4EA4}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{1C3EC6FB-407E-4007-95D8-EFDE35B025DE}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{5E880602-A850-4B92-A8F1-4DD8E5245D05}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{3EBEEBCE-9F60-4214-9C2B-528477464C2F}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{CBC96C1F-9C85-4E6E-9AA6-554A8F199DE5}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{F3F9A1E9-E5F1-4001-A6C5-679D9E23EFCD}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{13A8E850-673A-46FF-871E-3785BA88C85D}"/>
-    <hyperlink ref="A11" r:id="rId10" xr:uid="{A2F67EE0-32F2-474B-BCFE-1C8B72D9A5B2}"/>
-    <hyperlink ref="A12" r:id="rId11" xr:uid="{9D6477F5-E69C-4D79-B776-B469E6CF91F7}"/>
-    <hyperlink ref="A13" r:id="rId12" xr:uid="{0210A67F-8C03-4775-BA6C-E86020F05869}"/>
-    <hyperlink ref="A14" r:id="rId13" xr:uid="{47C17F50-9964-4ED3-B6D0-C77D4A34FC5A}"/>
-    <hyperlink ref="A15" r:id="rId14" xr:uid="{067430A8-550F-4A32-97CC-74BD3CC02A75}"/>
-    <hyperlink ref="A16" r:id="rId15" xr:uid="{63128FBD-EEBF-4A51-A57A-7EC073A278D0}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>